<commit_message>
visualisatie per tijdseenheid aangepast
</commit_message>
<xml_diff>
--- a/extra_data.xlsx
+++ b/extra_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dashboard_wormhotel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dashboard_wormhotel\wormhotel-california\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{700B2414-DB2D-4C8E-B2E7-79C05A5E42AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EE98F7-8D7F-47FE-9B0C-454676E1181D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Datum</t>
   </si>
@@ -90,20 +90,54 @@
     <t>g</t>
   </si>
   <si>
-    <t>g CO2</t>
-  </si>
-  <si>
     <t>kg</t>
+  </si>
+  <si>
+    <t>0.98 gram CO2 per kilogram GFT afval.</t>
+  </si>
+  <si>
+    <t>Vervoer</t>
+  </si>
+  <si>
+    <t>https://www.rvo.nl/sites/default/files/bijlagen/Bio-energie%20-%20Input%20-%20Groente-,%20fruit-%20en%20tuinafval%20(gft).pdf</t>
+  </si>
+  <si>
+    <t>Composteren ipv verbranden in een HVC reduceert uitstoot met 60 kg CO2 per ton GFT</t>
+  </si>
+  <si>
+    <t>Verbranding efficientie</t>
+  </si>
+  <si>
+    <t>Verbranden zelf</t>
+  </si>
+  <si>
+    <t>https://www.milieucentraal.nl/minder-afval/afval-scheiden/afval-scheiden-nut-en-fabels/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,14 +160,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:R29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,6 +489,9 @@
       <c r="B4">
         <v>743</v>
       </c>
+      <c r="J4" s="3" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -470,7 +511,7 @@
       <c r="J6" t="s">
         <v>5</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -545,6 +586,9 @@
       <c r="K12" t="s">
         <v>15</v>
       </c>
+      <c r="L12" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -575,11 +619,8 @@
       <c r="C20" t="s">
         <v>20</v>
       </c>
-      <c r="J20">
-        <v>8.5867599999999999</v>
-      </c>
-      <c r="K20" t="s">
-        <v>21</v>
+      <c r="J20" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -587,10 +628,48 @@
         <v>8.7620000000000005</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="J21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J24">
+        <v>60</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J25">
+        <v>60</v>
+      </c>
+      <c r="K25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J28" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="M6" r:id="rId1" xr:uid="{F07C2F8C-E1A6-44A9-BE76-62F9A79B814A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>